<commit_message>
gestione flags e args
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Cpeid</t>
   </si>
@@ -54,55 +54,31 @@
     <t>2019-08-13T07:37:21+0200</t>
   </si>
   <si>
+    <t>La Llorona - Le lacrime del male</t>
+  </si>
+  <si>
+    <t>voddashhttps.cb.ticdn.it</t>
+  </si>
+  <si>
+    <t>Europei a squadre</t>
+  </si>
+  <si>
+    <t>livetv0.cb.ticdn.it</t>
+  </si>
+  <si>
+    <t>2019-08-14T08:30:04+0200</t>
+  </si>
+  <si>
+    <t>2019-08-14T10:26:32+0200</t>
+  </si>
+  <si>
+    <t>Dragon Trainer - Il mondo nascosto</t>
+  </si>
+  <si>
     <t>2019-08-13T07:47:28+0200</t>
   </si>
   <si>
     <t>Alita - Angelo della battaglia</t>
-  </si>
-  <si>
-    <t>voddashhttps.cb.ticdn.it</t>
-  </si>
-  <si>
-    <t>La Llorona - Le lacrime del male</t>
-  </si>
-  <si>
-    <t>2019-08-10T08:17:15+0200</t>
-  </si>
-  <si>
-    <t>2019-08-10T08:19:56+0200</t>
-  </si>
-  <si>
-    <t>Europei a squadre</t>
-  </si>
-  <si>
-    <t>livetv0.cb.ticdn.it</t>
-  </si>
-  <si>
-    <t>2019-08-10T07:57:56+0200</t>
-  </si>
-  <si>
-    <t>2019-08-10T08:01:47+0200</t>
-  </si>
-  <si>
-    <t>L'uomo fedele</t>
-  </si>
-  <si>
-    <t>2019-08-10T04:28:30+0200</t>
-  </si>
-  <si>
-    <t>2019-08-10T07:35:46+0200</t>
-  </si>
-  <si>
-    <t>Black Sea</t>
-  </si>
-  <si>
-    <t>2019-08-10T02:05:06+0200</t>
-  </si>
-  <si>
-    <t>2019-08-10T04:08:54+0200</t>
-  </si>
-  <si>
-    <t>20 Mediaset</t>
   </si>
 </sst>
 </file>
@@ -119,7 +95,10 @@
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="00000000"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
@@ -222,7 +201,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -469,7 +448,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -529,22 +508,22 @@
         <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4">
@@ -554,26 +533,24 @@
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="C4" s="1" t="s"/>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5">
@@ -592,17 +569,17 @@
       <c r="E5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="1">
-        <v>3</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1">
+      <c r="F5">
         <v>1</v>
       </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
       <c r="I5" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6">
@@ -613,83 +590,25 @@
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="1">
+      <c r="F6">
         <v>1</v>
       </c>
-      <c r="G6" s="1">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1">
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
         <v>0</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>